<commit_message>
little changes in Agent and Policy
</commit_message>
<xml_diff>
--- a/Mappe1.xlsx
+++ b/Mappe1.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\projects\AlgoDat2\WorldDomination\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Jonas\ClionProjects\WorldDomination\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606ADD1B-2726-4EC7-AF6B-1B77AD913FA8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E422B5CF-9921-4968-B974-9928E6ABCC1D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="21600" windowHeight="11775" xr2:uid="{595E107C-C430-4B71-8FE3-5FD62108D455}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="465" windowWidth="21600" windowHeight="11775" activeTab="1" xr2:uid="{595E107C-C430-4B71-8FE3-5FD62108D455}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>index_first</t>
   </si>
@@ -66,17 +67,26 @@
     <t>x</t>
   </si>
   <si>
-    <t>e^1/(e^0+e^1+e^2+e^3)</t>
-  </si>
-  <si>
     <t>values</t>
+  </si>
+  <si>
+    <t>e^v1/(e^v0+e^v1+e^v2+e^v3)</t>
+  </si>
+  <si>
+    <t>exp(x1) = exp(1,64)</t>
+  </si>
+  <si>
+    <t>game</t>
+  </si>
+  <si>
+    <t>value function</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,8 +94,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -98,8 +121,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFC4B04"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -187,11 +234,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -233,6 +360,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -549,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BA0BAF2-BB2B-485C-ADDC-D32CE7892BE3}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,7 +975,7 @@
         <v>11</v>
       </c>
       <c r="H18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.25">
@@ -850,11 +986,11 @@
       <c r="E19" s="2"/>
       <c r="G19" s="12"/>
       <c r="H19" s="13">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="I19" s="14"/>
       <c r="J19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.25">
@@ -874,7 +1010,7 @@
         <v>12</v>
       </c>
       <c r="I20" s="17">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.25">
@@ -885,7 +1021,7 @@
       <c r="E21" s="2"/>
       <c r="G21" s="18"/>
       <c r="H21" s="19">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="I21" s="20"/>
     </row>
@@ -893,7 +1029,7 @@
       <c r="G23" s="3"/>
       <c r="H23" s="4">
         <f>2.71^H19</f>
-        <v>1</v>
+        <v>1.4900049676672025</v>
       </c>
       <c r="I23" s="5"/>
     </row>
@@ -905,38 +1041,41 @@
       <c r="H24" s="7"/>
       <c r="I24" s="8">
         <f>2.71^I20</f>
-        <v>1.1048337415228797</v>
+        <v>1.6462077633154328</v>
       </c>
       <c r="K24">
         <f>H23+I24+H25+G24</f>
-        <v>4.1048337415228797</v>
+        <v>5.626217698649838</v>
       </c>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G25" s="9"/>
       <c r="H25" s="10">
         <f>2.71^H21</f>
-        <v>1</v>
+        <v>1.4900049676672025</v>
       </c>
       <c r="I25" s="11"/>
+      <c r="J25" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="27" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G27" s="3"/>
       <c r="H27" s="4">
         <f>H23/$K$24</f>
-        <v>0.24361522608927963</v>
+        <v>0.26483244116642857</v>
       </c>
       <c r="I27" s="5"/>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G28" s="6">
         <f>G24/$K$24</f>
-        <v>0.24361522608927963</v>
+        <v>0.17773930081659955</v>
       </c>
       <c r="H28" s="7"/>
       <c r="I28" s="8">
         <f>I24/$K$24</f>
-        <v>0.26915432173216108</v>
+        <v>0.29259581685054326</v>
       </c>
       <c r="K28">
         <f>H27+I28+H29+G28</f>
@@ -947,9 +1086,108 @@
       <c r="G29" s="9"/>
       <c r="H29" s="10">
         <f>H25/$K$24</f>
-        <v>0.24361522608927963</v>
+        <v>0.26483244116642857</v>
       </c>
       <c r="I29" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B377EBD-2FF9-48DB-870C-C924D76FD37E}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="6" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" customWidth="1"/>
+    <col min="5" max="5" width="4.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="21"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="23">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <f>0.9*C2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="27"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="21">
+        <v>0</v>
+      </c>
+      <c r="C7" s="22">
+        <v>0</v>
+      </c>
+      <c r="D7" s="21">
+        <v>0</v>
+      </c>
+      <c r="E7" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="24">
+        <v>0</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="E8" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="27">
+        <v>0</v>
+      </c>
+      <c r="C9" s="28">
+        <v>0</v>
+      </c>
+      <c r="D9" s="28">
+        <v>0</v>
+      </c>
+      <c r="E9" s="29">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>